<commit_message>
last minute edits, refactoring, cleanup
</commit_message>
<xml_diff>
--- a/all_grid_search_metrics.xlsx
+++ b/all_grid_search_metrics.xlsx
@@ -498,16 +498,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5050505050505051</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5588512241054614</v>
+        <v>0.5056116722783389</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5050505050505051</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5514403292181069</v>
+        <v>0.5040388555973635</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -535,16 +535,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5635997988939165</v>
+        <v>0.5532598714416896</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="H3" t="n">
-        <v>0.544416597048176</v>
+        <v>0.5325015476927473</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -572,16 +572,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5858585858585859</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5864289374927673</v>
+        <v>0.5760546642899584</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5858585858585859</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5856049522478021</v>
+        <v>0.5756709956709957</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -611,16 +611,16 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6868686868686869</v>
+        <v>0.6565656565656566</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6877490122170974</v>
+        <v>0.6569617746088333</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6868686868686869</v>
+        <v>0.6565656565656566</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6866769151141918</v>
+        <v>0.6564955679241393</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -648,16 +648,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6060606060606061</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6104187374162142</v>
+        <v>0.5882076579750998</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6060606060606061</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6031476311850144</v>
+        <v>0.5840773324644293</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -688,16 +688,16 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.6262626262626263</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5053835053835054</v>
+        <v>0.6228474368009251</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.6262626262626263</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5061842548979082</v>
+        <v>0.5658616089325262</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -762,16 +762,16 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5797410726988192</v>
+        <v>0.5644007644007645</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5789569907216966</v>
+        <v>0.5614268772163509</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -801,16 +801,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6249640770188715</v>
+        <v>0.5886158886158885</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6170798898071626</v>
+        <v>0.582820688083846</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -838,16 +838,16 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5735274826183917</v>
+        <v>0.5617906756350692</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="H11" t="n">
-        <v>0.5640465374810726</v>
+        <v>0.5560579338357117</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -878,16 +878,16 @@
         <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4848484848484849</v>
+        <v>0.4747474747474748</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4845261121856866</v>
+        <v>0.4753494124922696</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4848484848484849</v>
+        <v>0.4747474747474748</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4846378965949738</v>
+        <v>0.4748546691403834</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -915,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5956198573097671</v>
+        <v>0.5752066115702479</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5959595959595959</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5955462976739573</v>
+        <v>0.5745394884033111</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -952,16 +952,16 @@
         <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6686291000841044</v>
+        <v>0.6398933249666641</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="H14" t="n">
-        <v>0.6642614163488301</v>
+        <v>0.6314557535487768</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -991,16 +991,16 @@
         <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7276094276094276</v>
+        <v>0.6475524475524476</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="H15" t="n">
-        <v>0.726770004189359</v>
+        <v>0.6323232323232323</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1028,16 +1028,16 @@
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6262626262626263</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6450020567667627</v>
+        <v>0.6354453627180899</v>
       </c>
       <c r="G16" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6262626262626263</v>
       </c>
       <c r="H16" t="n">
-        <v>0.6272650814282438</v>
+        <v>0.6156148378370602</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1068,16 +1068,16 @@
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7676767676767676</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7509157509157508</v>
+        <v>0.7348484848484849</v>
       </c>
       <c r="G17" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7676767676767676</v>
       </c>
       <c r="H17" t="n">
-        <v>0.7329317269076305</v>
+        <v>0.7337954479058773</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1108,13 +1108,13 @@
         <v>0.7575757575757576</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.722048066875653</v>
       </c>
       <c r="G18" t="n">
         <v>0.7575757575757576</v>
       </c>
       <c r="H18" t="n">
-        <v>0.7332535885167464</v>
+        <v>0.7261503928170594</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6464646464646465</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6166666666666666</v>
+        <v>0.6063432024694578</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6464646464646465</v>
       </c>
       <c r="H19" t="n">
-        <v>0.6376390904692792</v>
+        <v>0.6241661605961747</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1332,16 +1332,16 @@
         <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6262626262626263</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="F24" t="n">
-        <v>0.628300549353181</v>
+        <v>0.6394219741570457</v>
       </c>
       <c r="G24" t="n">
-        <v>0.6262626262626263</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="H24" t="n">
-        <v>0.6241131661692408</v>
+        <v>0.6336700336700336</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1371,16 +1371,16 @@
         <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>0.494949494949495</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F25" t="n">
-        <v>0.4646464646464646</v>
+        <v>0.5408432147562582</v>
       </c>
       <c r="G25" t="n">
-        <v>0.494949494949495</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="H25" t="n">
-        <v>0.3802461232038697</v>
+        <v>0.4050362782757149</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1408,16 +1408,16 @@
         <v>4</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5757575757575758</v>
+        <v>0.5656565656565656</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5965929565929565</v>
+        <v>0.5813243073517046</v>
       </c>
       <c r="G26" t="n">
-        <v>0.5757575757575758</v>
+        <v>0.5656565656565656</v>
       </c>
       <c r="H26" t="n">
-        <v>0.5480172254365803</v>
+        <v>0.5396665845446332</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1451,16 +1451,16 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6161616161616161</v>
+        <v>0.5959595959595959</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6243714103938435</v>
+        <v>0.6085378673613967</v>
       </c>
       <c r="G27" t="n">
-        <v>0.6161616161616161</v>
+        <v>0.5959595959595959</v>
       </c>
       <c r="H27" t="n">
-        <v>0.6109274563820019</v>
+        <v>0.5858332700437965</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1494,16 +1494,16 @@
         <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6295049258012221</v>
+        <v>0.5845615408025738</v>
       </c>
       <c r="G28" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="H28" t="n">
-        <v>0.5959695476936857</v>
+        <v>0.5587114142545274</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1537,16 +1537,16 @@
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6161616161616161</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6705128205128206</v>
+        <v>0.6173600410888547</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6161616161616161</v>
       </c>
       <c r="H29" t="n">
-        <v>0.6629388008698355</v>
+        <v>0.61267217630854</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1580,16 +1580,16 @@
         <v>3</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7373737373737373</v>
+        <v>0.7474747474747475</v>
       </c>
       <c r="F30" t="n">
-        <v>0.634768740031898</v>
+        <v>0.6772404900064475</v>
       </c>
       <c r="G30" t="n">
-        <v>0.7373737373737373</v>
+        <v>0.7474747474747475</v>
       </c>
       <c r="H30" t="n">
-        <v>0.6590272472625414</v>
+        <v>0.678946164357305</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1626,13 +1626,13 @@
         <v>0.6060606060606061</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6332343455631126</v>
+        <v>0.6588991177598773</v>
       </c>
       <c r="G31" t="n">
         <v>0.6060606060606061</v>
       </c>
       <c r="H31" t="n">
-        <v>0.5824882976102489</v>
+        <v>0.5675562500638335</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>

</xml_diff>